<commit_message>
finished R script in Markdown to add Delphin LPG *.lpm measurement files to xlsx-Database.
</commit_message>
<xml_diff>
--- a/LPG_Temperatur_DB.xlsx
+++ b/LPG_Temperatur_DB.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t xml:space="preserve">datetime</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t xml:space="preserve">U110_T_BD0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15.06.2020 17:09:01</t>
   </si>
   <si>
     <t xml:space="preserve">APOLLO G2 SKII Cityline</t>
@@ -271,7 +268,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="dd.mm.yy hh:mm:ss"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -306,13 +306,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,7 +693,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="15.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="16.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="13.71" hidden="0" customWidth="1"/>
@@ -986,223 +990,223 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="n">
+        <v>43997.7145949074</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="1" t="n">
+      <c r="J2" s="2" t="n">
         <v>23.439</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="K2" s="2" t="n">
         <v>207.3</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="L2" s="2" t="n">
         <v>0.181</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="M2" s="2" t="n">
         <v>36.9</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="N2" s="2" t="n">
         <v>207.5</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="O2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P2" s="1" t="n">
+      <c r="P2" s="2" t="n">
         <v>31.212</v>
       </c>
-      <c r="Q2" s="1" t="n">
+      <c r="Q2" s="2" t="n">
         <v>56.304</v>
       </c>
-      <c r="R2" s="1" t="n">
+      <c r="R2" s="2" t="n">
         <v>55.289</v>
       </c>
-      <c r="S2" s="1" t="n">
+      <c r="S2" s="2" t="n">
         <v>57.598</v>
       </c>
-      <c r="T2" s="1" t="n">
+      <c r="T2" s="2" t="n">
         <v>37.492</v>
       </c>
-      <c r="U2" s="1" t="n">
+      <c r="U2" s="2" t="n">
         <v>36.625</v>
       </c>
-      <c r="V2" s="1" t="n">
+      <c r="V2" s="2" t="n">
         <v>40.142</v>
       </c>
-      <c r="W2" s="1" t="n">
+      <c r="W2" s="2" t="n">
         <v>38.508</v>
       </c>
-      <c r="X2" s="1" t="n">
+      <c r="X2" s="2" t="n">
         <v>35.041</v>
       </c>
-      <c r="Y2" s="1" t="n">
+      <c r="Y2" s="2" t="n">
         <v>32.833</v>
       </c>
-      <c r="Z2" s="1" t="n">
+      <c r="Z2" s="2" t="n">
         <v>23.607</v>
       </c>
-      <c r="AA2" s="1" t="n">
+      <c r="AA2" s="2" t="n">
         <v>229.3</v>
       </c>
-      <c r="AB2" s="1" t="n">
+      <c r="AB2" s="2" t="n">
         <v>0.164</v>
       </c>
-      <c r="AC2" s="1" t="n">
+      <c r="AC2" s="2" t="n">
         <v>36.9</v>
       </c>
-      <c r="AD2" s="1" t="n">
+      <c r="AD2" s="2" t="n">
         <v>230</v>
       </c>
-      <c r="AE2" s="1" t="n">
+      <c r="AE2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AF2" s="1" t="n">
+      <c r="AF2" s="2" t="n">
         <v>31.58</v>
       </c>
-      <c r="AG2" s="1" t="n">
+      <c r="AG2" s="2" t="n">
         <v>56.54</v>
       </c>
-      <c r="AH2" s="1" t="n">
+      <c r="AH2" s="2" t="n">
         <v>55.396</v>
       </c>
-      <c r="AI2" s="1" t="n">
+      <c r="AI2" s="2" t="n">
         <v>57.606</v>
       </c>
-      <c r="AJ2" s="1" t="n">
+      <c r="AJ2" s="2" t="n">
         <v>37.667</v>
       </c>
-      <c r="AK2" s="1" t="n">
+      <c r="AK2" s="2" t="n">
         <v>36.762</v>
       </c>
-      <c r="AL2" s="1" t="n">
+      <c r="AL2" s="2" t="n">
         <v>41.095</v>
       </c>
-      <c r="AM2" s="1" t="n">
+      <c r="AM2" s="2" t="n">
         <v>39.124</v>
       </c>
-      <c r="AN2" s="1" t="n">
+      <c r="AN2" s="2" t="n">
         <v>35.083</v>
       </c>
-      <c r="AO2" s="1" t="n">
+      <c r="AO2" s="2" t="n">
         <v>32.934</v>
       </c>
-      <c r="AP2" s="1" t="n">
+      <c r="AP2" s="2" t="n">
         <v>23.76</v>
       </c>
-      <c r="AQ2" s="1" t="n">
+      <c r="AQ2" s="2" t="n">
         <v>244</v>
       </c>
-      <c r="AR2" s="1" t="n">
+      <c r="AR2" s="2" t="n">
         <v>0.155</v>
       </c>
-      <c r="AS2" s="1" t="n">
+      <c r="AS2" s="2" t="n">
         <v>36.9</v>
       </c>
-      <c r="AT2" s="1" t="n">
+      <c r="AT2" s="2" t="n">
         <v>242.9</v>
       </c>
-      <c r="AU2" s="1" t="n">
+      <c r="AU2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AV2" s="1" t="n">
+      <c r="AV2" s="2" t="n">
         <v>31.735</v>
       </c>
-      <c r="AW2" s="1" t="n">
+      <c r="AW2" s="2" t="n">
         <v>56.638</v>
       </c>
-      <c r="AX2" s="1" t="n">
+      <c r="AX2" s="2" t="n">
         <v>55.55</v>
       </c>
-      <c r="AY2" s="1" t="n">
+      <c r="AY2" s="2" t="n">
         <v>57.655</v>
       </c>
-      <c r="AZ2" s="1" t="n">
+      <c r="AZ2" s="2" t="n">
         <v>37.851</v>
       </c>
-      <c r="BA2" s="1" t="n">
+      <c r="BA2" s="2" t="n">
         <v>36.885</v>
       </c>
-      <c r="BB2" s="1" t="n">
+      <c r="BB2" s="2" t="n">
         <v>41.77</v>
       </c>
-      <c r="BC2" s="1" t="n">
+      <c r="BC2" s="2" t="n">
         <v>39.443</v>
       </c>
-      <c r="BD2" s="1" t="n">
+      <c r="BD2" s="2" t="n">
         <v>35.273</v>
       </c>
-      <c r="BE2" s="1" t="n">
+      <c r="BE2" s="2" t="n">
         <v>33.184</v>
       </c>
-      <c r="BF2" s="1" t="n">
+      <c r="BF2" s="2" t="n">
         <v>23.901</v>
       </c>
-      <c r="BG2" s="1" t="n">
+      <c r="BG2" s="2" t="n">
         <v>253.1</v>
       </c>
-      <c r="BH2" s="1" t="n">
+      <c r="BH2" s="2" t="n">
         <v>0.149</v>
       </c>
-      <c r="BI2" s="1" t="n">
+      <c r="BI2" s="2" t="n">
         <v>36.7</v>
       </c>
-      <c r="BJ2" s="1" t="n">
+      <c r="BJ2" s="2" t="n">
         <v>254.3</v>
       </c>
-      <c r="BK2" s="1" t="n">
+      <c r="BK2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BL2" s="1" t="n">
+      <c r="BL2" s="2" t="n">
         <v>31.865</v>
       </c>
-      <c r="BM2" s="1" t="n">
+      <c r="BM2" s="2" t="n">
         <v>56.797</v>
       </c>
-      <c r="BN2" s="1" t="n">
+      <c r="BN2" s="2" t="n">
         <v>55.617</v>
       </c>
-      <c r="BO2" s="1" t="n">
+      <c r="BO2" s="2" t="n">
         <v>57.632</v>
       </c>
-      <c r="BP2" s="1" t="n">
+      <c r="BP2" s="2" t="n">
         <v>37.969</v>
       </c>
-      <c r="BQ2" s="1" t="n">
+      <c r="BQ2" s="2" t="n">
         <v>37.039</v>
       </c>
-      <c r="BR2" s="1" t="n">
+      <c r="BR2" s="2" t="n">
         <v>42.098</v>
       </c>
-      <c r="BS2" s="1" t="n">
+      <c r="BS2" s="2" t="n">
         <v>39.645</v>
       </c>
-      <c r="BT2" s="1" t="n">
+      <c r="BT2" s="2" t="n">
         <v>35.304</v>
       </c>
-      <c r="BU2" s="1" t="n">
+      <c r="BU2" s="2" t="n">
         <v>33.127</v>
       </c>
     </row>

</xml_diff>

<commit_message>
converted R Markdown to normal R script
</commit_message>
<xml_diff>
--- a/LPG_Temperatur_DB.xlsx
+++ b/LPG_Temperatur_DB.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t xml:space="preserve">datetime</t>
   </si>
@@ -41,6 +41,96 @@
     <t xml:space="preserve">notes3</t>
   </si>
   <si>
+    <t xml:space="preserve">U100_Raumtemperatur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_UNenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_INenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_PNenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_U_Lampe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_VG_BWQuotient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_T_BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_T_AK_S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_T_D12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_T_EVG_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_T_LED_1E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_T_LED_1M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_T_LOH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_T_LOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_T_ESB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_Raumtemperatur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_UNenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_INenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_PNenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_U_Lampe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_VG_BWQuotient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_T_BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_T_AK_S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_T_D12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_T_EVG_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_T_LED_1E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_T_LED_1M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_T_LOH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_T_LOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_T_ESB</t>
+  </si>
+  <si>
     <t xml:space="preserve">U090_Raumtemperatur</t>
   </si>
   <si>
@@ -65,178 +155,139 @@
     <t xml:space="preserve">U090_T_AK_S</t>
   </si>
   <si>
+    <t xml:space="preserve">U090_T_D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U090_T_EVG_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U090_T_LED_1E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U090_T_LED_1M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U090_T_LOH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U090_T_LOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U100_T_D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_Raumtemperatur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_UNenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_INenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_PNenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_U_Lampe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_VG_BWQuotient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_T_BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_T_AK_S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_T_D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_T_EVG_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_T_LED_1E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_T_LED_1M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_T_LOH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U106_T_LOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U110_T_D10</t>
+  </si>
+  <si>
     <t xml:space="preserve">U090_T_D12</t>
   </si>
   <si>
-    <t xml:space="preserve">U090_T_EVG_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U090_T_LED_1E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U090_T_LED_1M</t>
-  </si>
-  <si>
     <t xml:space="preserve">U090_T_ESB</t>
   </si>
   <si>
     <t xml:space="preserve">U090_T_SPC</t>
   </si>
   <si>
-    <t xml:space="preserve">U090_T_LOH</t>
-  </si>
-  <si>
     <t xml:space="preserve">U090_T_BD0</t>
   </si>
   <si>
-    <t xml:space="preserve">U100_Raumtemperatur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_UNenn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_INenn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_PNenn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_U_Lampe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_VG_BWQuotient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_T_BD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_T_AK_S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_T_D12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_T_EVG_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_T_LED_1E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_T_LED_1M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U100_T_ESB</t>
-  </si>
-  <si>
     <t xml:space="preserve">U100_T_SPC</t>
   </si>
   <si>
-    <t xml:space="preserve">U100_T_LOH</t>
-  </si>
-  <si>
     <t xml:space="preserve">U100_T_BD0</t>
   </si>
   <si>
-    <t xml:space="preserve">U106_Raumtemperatur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U106_UNenn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U106_INenn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U106_PNenn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U106_U_Lampe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U106_VG_BWQuotient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U106_T_BD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U106_T_AK_S</t>
-  </si>
-  <si>
     <t xml:space="preserve">U106_T_D12</t>
   </si>
   <si>
-    <t xml:space="preserve">U106_T_EVG_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U106_T_LED_1E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U106_T_LED_1M</t>
-  </si>
-  <si>
     <t xml:space="preserve">U106_T_ESB</t>
   </si>
   <si>
     <t xml:space="preserve">U106_T_SPC</t>
   </si>
   <si>
-    <t xml:space="preserve">U106_T_LOH</t>
-  </si>
-  <si>
     <t xml:space="preserve">U106_T_BD0</t>
   </si>
   <si>
-    <t xml:space="preserve">U110_Raumtemperatur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_UNenn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_INenn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_PNenn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_U_Lampe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_VG_BWQuotient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_T_BD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_T_AK_S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_T_D12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_T_EVG_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_T_LED_1E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_T_LED_1M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U110_T_ESB</t>
-  </si>
-  <si>
     <t xml:space="preserve">U110_T_SPC</t>
   </si>
   <si>
-    <t xml:space="preserve">U110_T_LOH</t>
-  </si>
-  <si>
     <t xml:space="preserve">U110_T_BD0</t>
   </si>
   <si>
+    <t xml:space="preserve">Apollo G2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED Anbauleuchte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an die Decke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ohne anormalen Betrieb / without abnormal operation
+mit DV 4x2,5mm² = 16A / with through-wiring 4x2,5mm² = 16A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPR 2125/2-288 36T5 840 DA 0.375A2 Pw PO E
+1x Osram Oti DX 100/220...240/700 D NFC IND L
+2x2x LLE 24x560mm 4000lm 840 HV ADV5
+1x ESB-6K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I_DC: 1x 0.375A
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">APOLLO G2 SKII Cityline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED Anbauleuchte</t>
   </si>
   <si>
     <t xml:space="preserve">Deckenmontage</t>
@@ -261,6 +312,30 @@
   </si>
   <si>
     <t xml:space="preserve">I_DC: 1x 0.750A
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAUNUS v20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED Einbauleuchte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deckeneinbau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ohne anormalen Betrieb / without abnormal operation
+ohne DV / without through wiring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPR DD 2000/1-192 48O6 940 FO 0.650A1 TbM PC
+1x Xitanium 36W 0.3-1A 54V 230V
+2x PL-LIN-Z6 4000-940 560X20-LV
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I_DC: 1x 1.10A
 </t>
   </si>
 </sst>
@@ -270,7 +345,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="166" formatCode="yyyy/mm/dd hh:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="dd.mm.yy hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="dd.mm.yyyy hh:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -327,9 +402,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:BU2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:BU2"/>
-  <tableColumns count="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:CC4" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:CC4"/>
+  <tableColumns count="81">
     <tableColumn id="1" name="datetime"/>
     <tableColumn id="2" name="family"/>
     <tableColumn id="3" name="luminaire"/>
@@ -339,70 +414,78 @@
     <tableColumn id="7" name="notes1"/>
     <tableColumn id="8" name="notes2"/>
     <tableColumn id="9" name="notes3"/>
-    <tableColumn id="10" name="U090_Raumtemperatur"/>
-    <tableColumn id="11" name="U090_UNenn"/>
-    <tableColumn id="12" name="U090_INenn"/>
-    <tableColumn id="13" name="U090_PNenn"/>
-    <tableColumn id="14" name="U090_U_Lampe"/>
-    <tableColumn id="15" name="U090_VG_BWQuotient"/>
-    <tableColumn id="16" name="U090_T_BD"/>
-    <tableColumn id="17" name="U090_T_AK_S"/>
-    <tableColumn id="18" name="U090_T_D12"/>
-    <tableColumn id="19" name="U090_T_EVG_1"/>
-    <tableColumn id="20" name="U090_T_LED_1E"/>
-    <tableColumn id="21" name="U090_T_LED_1M"/>
-    <tableColumn id="22" name="U090_T_ESB"/>
-    <tableColumn id="23" name="U090_T_SPC"/>
-    <tableColumn id="24" name="U090_T_LOH"/>
-    <tableColumn id="25" name="U090_T_BD0"/>
-    <tableColumn id="26" name="U100_Raumtemperatur"/>
-    <tableColumn id="27" name="U100_UNenn"/>
-    <tableColumn id="28" name="U100_INenn"/>
-    <tableColumn id="29" name="U100_PNenn"/>
-    <tableColumn id="30" name="U100_U_Lampe"/>
-    <tableColumn id="31" name="U100_VG_BWQuotient"/>
-    <tableColumn id="32" name="U100_T_BD"/>
-    <tableColumn id="33" name="U100_T_AK_S"/>
-    <tableColumn id="34" name="U100_T_D12"/>
-    <tableColumn id="35" name="U100_T_EVG_1"/>
-    <tableColumn id="36" name="U100_T_LED_1E"/>
-    <tableColumn id="37" name="U100_T_LED_1M"/>
-    <tableColumn id="38" name="U100_T_ESB"/>
-    <tableColumn id="39" name="U100_T_SPC"/>
-    <tableColumn id="40" name="U100_T_LOH"/>
-    <tableColumn id="41" name="U100_T_BD0"/>
-    <tableColumn id="42" name="U106_Raumtemperatur"/>
-    <tableColumn id="43" name="U106_UNenn"/>
-    <tableColumn id="44" name="U106_INenn"/>
-    <tableColumn id="45" name="U106_PNenn"/>
-    <tableColumn id="46" name="U106_U_Lampe"/>
-    <tableColumn id="47" name="U106_VG_BWQuotient"/>
-    <tableColumn id="48" name="U106_T_BD"/>
-    <tableColumn id="49" name="U106_T_AK_S"/>
-    <tableColumn id="50" name="U106_T_D12"/>
-    <tableColumn id="51" name="U106_T_EVG_1"/>
-    <tableColumn id="52" name="U106_T_LED_1E"/>
-    <tableColumn id="53" name="U106_T_LED_1M"/>
-    <tableColumn id="54" name="U106_T_ESB"/>
-    <tableColumn id="55" name="U106_T_SPC"/>
-    <tableColumn id="56" name="U106_T_LOH"/>
-    <tableColumn id="57" name="U106_T_BD0"/>
-    <tableColumn id="58" name="U110_Raumtemperatur"/>
-    <tableColumn id="59" name="U110_UNenn"/>
-    <tableColumn id="60" name="U110_INenn"/>
-    <tableColumn id="61" name="U110_PNenn"/>
-    <tableColumn id="62" name="U110_U_Lampe"/>
-    <tableColumn id="63" name="U110_VG_BWQuotient"/>
-    <tableColumn id="64" name="U110_T_BD"/>
-    <tableColumn id="65" name="U110_T_AK_S"/>
-    <tableColumn id="66" name="U110_T_D12"/>
-    <tableColumn id="67" name="U110_T_EVG_1"/>
-    <tableColumn id="68" name="U110_T_LED_1E"/>
-    <tableColumn id="69" name="U110_T_LED_1M"/>
-    <tableColumn id="70" name="U110_T_ESB"/>
-    <tableColumn id="71" name="U110_T_SPC"/>
-    <tableColumn id="72" name="U110_T_LOH"/>
-    <tableColumn id="73" name="U110_T_BD0"/>
+    <tableColumn id="10" name="U100_Raumtemperatur"/>
+    <tableColumn id="11" name="U100_UNenn"/>
+    <tableColumn id="12" name="U100_INenn"/>
+    <tableColumn id="13" name="U100_PNenn"/>
+    <tableColumn id="14" name="U100_U_Lampe"/>
+    <tableColumn id="15" name="U100_VG_BWQuotient"/>
+    <tableColumn id="16" name="U100_T_BD"/>
+    <tableColumn id="17" name="U100_T_AK_S"/>
+    <tableColumn id="18" name="U100_T_D12"/>
+    <tableColumn id="19" name="U100_T_EVG_1"/>
+    <tableColumn id="20" name="U100_T_LED_1E"/>
+    <tableColumn id="21" name="U100_T_LED_1M"/>
+    <tableColumn id="22" name="U100_T_LOH"/>
+    <tableColumn id="23" name="U100_T_LOV"/>
+    <tableColumn id="24" name="U100_T_ESB"/>
+    <tableColumn id="25" name="U110_Raumtemperatur"/>
+    <tableColumn id="26" name="U110_UNenn"/>
+    <tableColumn id="27" name="U110_INenn"/>
+    <tableColumn id="28" name="U110_PNenn"/>
+    <tableColumn id="29" name="U110_U_Lampe"/>
+    <tableColumn id="30" name="U110_VG_BWQuotient"/>
+    <tableColumn id="31" name="U110_T_BD"/>
+    <tableColumn id="32" name="U110_T_AK_S"/>
+    <tableColumn id="33" name="U110_T_D12"/>
+    <tableColumn id="34" name="U110_T_EVG_1"/>
+    <tableColumn id="35" name="U110_T_LED_1E"/>
+    <tableColumn id="36" name="U110_T_LED_1M"/>
+    <tableColumn id="37" name="U110_T_LOH"/>
+    <tableColumn id="38" name="U110_T_LOV"/>
+    <tableColumn id="39" name="U110_T_ESB"/>
+    <tableColumn id="40" name="U090_Raumtemperatur"/>
+    <tableColumn id="41" name="U090_UNenn"/>
+    <tableColumn id="42" name="U090_INenn"/>
+    <tableColumn id="43" name="U090_PNenn"/>
+    <tableColumn id="44" name="U090_U_Lampe"/>
+    <tableColumn id="45" name="U090_VG_BWQuotient"/>
+    <tableColumn id="46" name="U090_T_BD"/>
+    <tableColumn id="47" name="U090_T_AK_S"/>
+    <tableColumn id="48" name="U090_T_D10"/>
+    <tableColumn id="49" name="U090_T_EVG_1"/>
+    <tableColumn id="50" name="U090_T_LED_1E"/>
+    <tableColumn id="51" name="U090_T_LED_1M"/>
+    <tableColumn id="52" name="U090_T_LOH"/>
+    <tableColumn id="53" name="U090_T_LOV"/>
+    <tableColumn id="54" name="U100_T_D10"/>
+    <tableColumn id="55" name="U106_Raumtemperatur"/>
+    <tableColumn id="56" name="U106_UNenn"/>
+    <tableColumn id="57" name="U106_INenn"/>
+    <tableColumn id="58" name="U106_PNenn"/>
+    <tableColumn id="59" name="U106_U_Lampe"/>
+    <tableColumn id="60" name="U106_VG_BWQuotient"/>
+    <tableColumn id="61" name="U106_T_BD"/>
+    <tableColumn id="62" name="U106_T_AK_S"/>
+    <tableColumn id="63" name="U106_T_D10"/>
+    <tableColumn id="64" name="U106_T_EVG_1"/>
+    <tableColumn id="65" name="U106_T_LED_1E"/>
+    <tableColumn id="66" name="U106_T_LED_1M"/>
+    <tableColumn id="67" name="U106_T_LOH"/>
+    <tableColumn id="68" name="U106_T_LOV"/>
+    <tableColumn id="69" name="U110_T_D10"/>
+    <tableColumn id="70" name="U090_T_D12"/>
+    <tableColumn id="71" name="U090_T_ESB"/>
+    <tableColumn id="72" name="U090_T_SPC"/>
+    <tableColumn id="73" name="U090_T_BD0"/>
+    <tableColumn id="74" name="U100_T_SPC"/>
+    <tableColumn id="75" name="U100_T_BD0"/>
+    <tableColumn id="76" name="U106_T_D12"/>
+    <tableColumn id="77" name="U106_T_ESB"/>
+    <tableColumn id="78" name="U106_T_SPC"/>
+    <tableColumn id="79" name="U106_T_BD0"/>
+    <tableColumn id="80" name="U110_T_SPC"/>
+    <tableColumn id="81" name="U110_T_BD0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -693,9 +776,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="15.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="16.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="17.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="13.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="3.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="3.71" hidden="0" customWidth="1"/>
@@ -717,55 +800,63 @@
     <col min="22" max="22" width="10.71" hidden="0" customWidth="1"/>
     <col min="23" max="23" width="10.71" hidden="0" customWidth="1"/>
     <col min="24" max="24" width="10.71" hidden="0" customWidth="1"/>
-    <col min="25" max="25" width="10.71" hidden="0" customWidth="1"/>
-    <col min="26" max="26" width="19.71" hidden="0" customWidth="1"/>
+    <col min="25" max="25" width="19.71" hidden="0" customWidth="1"/>
+    <col min="26" max="26" width="10.71" hidden="0" customWidth="1"/>
     <col min="27" max="27" width="10.71" hidden="0" customWidth="1"/>
     <col min="28" max="28" width="10.71" hidden="0" customWidth="1"/>
-    <col min="29" max="29" width="10.71" hidden="0" customWidth="1"/>
-    <col min="30" max="30" width="12.71" hidden="0" customWidth="1"/>
-    <col min="31" max="31" width="18.71" hidden="0" customWidth="1"/>
-    <col min="32" max="32" width="9.71" hidden="0" customWidth="1"/>
-    <col min="33" max="33" width="11.71" hidden="0" customWidth="1"/>
-    <col min="34" max="34" width="10.71" hidden="0" customWidth="1"/>
-    <col min="35" max="35" width="12.71" hidden="0" customWidth="1"/>
+    <col min="29" max="29" width="12.71" hidden="0" customWidth="1"/>
+    <col min="30" max="30" width="18.71" hidden="0" customWidth="1"/>
+    <col min="31" max="31" width="9.71" hidden="0" customWidth="1"/>
+    <col min="32" max="32" width="11.71" hidden="0" customWidth="1"/>
+    <col min="33" max="33" width="10.71" hidden="0" customWidth="1"/>
+    <col min="34" max="34" width="12.71" hidden="0" customWidth="1"/>
+    <col min="35" max="35" width="13.71" hidden="0" customWidth="1"/>
     <col min="36" max="36" width="13.71" hidden="0" customWidth="1"/>
-    <col min="37" max="37" width="13.71" hidden="0" customWidth="1"/>
+    <col min="37" max="37" width="10.71" hidden="0" customWidth="1"/>
     <col min="38" max="38" width="10.71" hidden="0" customWidth="1"/>
     <col min="39" max="39" width="10.71" hidden="0" customWidth="1"/>
-    <col min="40" max="40" width="10.71" hidden="0" customWidth="1"/>
+    <col min="40" max="40" width="19.71" hidden="0" customWidth="1"/>
     <col min="41" max="41" width="10.71" hidden="0" customWidth="1"/>
-    <col min="42" max="42" width="19.71" hidden="0" customWidth="1"/>
+    <col min="42" max="42" width="10.71" hidden="0" customWidth="1"/>
     <col min="43" max="43" width="10.71" hidden="0" customWidth="1"/>
-    <col min="44" max="44" width="10.71" hidden="0" customWidth="1"/>
-    <col min="45" max="45" width="10.71" hidden="0" customWidth="1"/>
-    <col min="46" max="46" width="12.71" hidden="0" customWidth="1"/>
-    <col min="47" max="47" width="18.71" hidden="0" customWidth="1"/>
-    <col min="48" max="48" width="9.71" hidden="0" customWidth="1"/>
-    <col min="49" max="49" width="11.71" hidden="0" customWidth="1"/>
-    <col min="50" max="50" width="10.71" hidden="0" customWidth="1"/>
-    <col min="51" max="51" width="12.71" hidden="0" customWidth="1"/>
-    <col min="52" max="52" width="13.71" hidden="0" customWidth="1"/>
-    <col min="53" max="53" width="13.71" hidden="0" customWidth="1"/>
+    <col min="44" max="44" width="12.71" hidden="0" customWidth="1"/>
+    <col min="45" max="45" width="18.71" hidden="0" customWidth="1"/>
+    <col min="46" max="46" width="9.71" hidden="0" customWidth="1"/>
+    <col min="47" max="47" width="11.71" hidden="0" customWidth="1"/>
+    <col min="48" max="48" width="10.71" hidden="0" customWidth="1"/>
+    <col min="49" max="49" width="12.71" hidden="0" customWidth="1"/>
+    <col min="50" max="50" width="13.71" hidden="0" customWidth="1"/>
+    <col min="51" max="51" width="13.71" hidden="0" customWidth="1"/>
+    <col min="52" max="52" width="10.71" hidden="0" customWidth="1"/>
+    <col min="53" max="53" width="10.71" hidden="0" customWidth="1"/>
     <col min="54" max="54" width="10.71" hidden="0" customWidth="1"/>
-    <col min="55" max="55" width="10.71" hidden="0" customWidth="1"/>
+    <col min="55" max="55" width="19.71" hidden="0" customWidth="1"/>
     <col min="56" max="56" width="10.71" hidden="0" customWidth="1"/>
     <col min="57" max="57" width="10.71" hidden="0" customWidth="1"/>
-    <col min="58" max="58" width="19.71" hidden="0" customWidth="1"/>
-    <col min="59" max="59" width="10.71" hidden="0" customWidth="1"/>
-    <col min="60" max="60" width="10.71" hidden="0" customWidth="1"/>
-    <col min="61" max="61" width="10.71" hidden="0" customWidth="1"/>
-    <col min="62" max="62" width="12.71" hidden="0" customWidth="1"/>
-    <col min="63" max="63" width="18.71" hidden="0" customWidth="1"/>
-    <col min="64" max="64" width="9.71" hidden="0" customWidth="1"/>
-    <col min="65" max="65" width="11.71" hidden="0" customWidth="1"/>
-    <col min="66" max="66" width="10.71" hidden="0" customWidth="1"/>
-    <col min="67" max="67" width="12.71" hidden="0" customWidth="1"/>
-    <col min="68" max="68" width="13.71" hidden="0" customWidth="1"/>
-    <col min="69" max="69" width="13.71" hidden="0" customWidth="1"/>
+    <col min="58" max="58" width="10.71" hidden="0" customWidth="1"/>
+    <col min="59" max="59" width="12.71" hidden="0" customWidth="1"/>
+    <col min="60" max="60" width="18.71" hidden="0" customWidth="1"/>
+    <col min="61" max="61" width="9.71" hidden="0" customWidth="1"/>
+    <col min="62" max="62" width="11.71" hidden="0" customWidth="1"/>
+    <col min="63" max="63" width="10.71" hidden="0" customWidth="1"/>
+    <col min="64" max="64" width="12.71" hidden="0" customWidth="1"/>
+    <col min="65" max="65" width="13.71" hidden="0" customWidth="1"/>
+    <col min="66" max="66" width="13.71" hidden="0" customWidth="1"/>
+    <col min="67" max="67" width="10.71" hidden="0" customWidth="1"/>
+    <col min="68" max="68" width="10.71" hidden="0" customWidth="1"/>
+    <col min="69" max="69" width="10.71" hidden="0" customWidth="1"/>
     <col min="70" max="70" width="10.71" hidden="0" customWidth="1"/>
     <col min="71" max="71" width="10.71" hidden="0" customWidth="1"/>
     <col min="72" max="72" width="10.71" hidden="0" customWidth="1"/>
     <col min="73" max="73" width="10.71" hidden="0" customWidth="1"/>
+    <col min="74" max="74" width="10.71" hidden="0" customWidth="1"/>
+    <col min="75" max="75" width="10.71" hidden="0" customWidth="1"/>
+    <col min="76" max="76" width="10.71" hidden="0" customWidth="1"/>
+    <col min="77" max="77" width="10.71" hidden="0" customWidth="1"/>
+    <col min="78" max="78" width="10.71" hidden="0" customWidth="1"/>
+    <col min="79" max="79" width="10.71" hidden="0" customWidth="1"/>
+    <col min="80" max="80" width="10.71" hidden="0" customWidth="1"/>
+    <col min="81" max="81" width="10.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -988,227 +1079,633 @@
       <c r="BU1" t="s">
         <v>72</v>
       </c>
+      <c r="BV1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="n">
-        <v>43997.7145949074</v>
+        <v>44433.6224652778</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>23.439</v>
+        <v>26.875</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>207.3</v>
+        <v>229.6</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>0.181</v>
+        <v>0.472</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>36.9</v>
+        <v>106</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>207.5</v>
+        <v>230.9</v>
       </c>
       <c r="O2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="P2" s="2" t="n">
+        <v>40.76</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>56.147</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>56.146</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>61.609</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>58.856</v>
+      </c>
+      <c r="U2" s="2" t="n">
+        <v>61.527</v>
+      </c>
+      <c r="V2" s="2" t="n">
+        <v>50.598</v>
+      </c>
+      <c r="W2" s="2" t="n">
+        <v>42.901</v>
+      </c>
+      <c r="X2" s="2" t="n">
+        <v>44.773</v>
+      </c>
+      <c r="Y2" s="2" t="n">
+        <v>27.002</v>
+      </c>
+      <c r="Z2" s="2" t="n">
+        <v>252</v>
+      </c>
+      <c r="AA2" s="2" t="n">
+        <v>0.433</v>
+      </c>
+      <c r="AB2" s="2" t="n">
+        <v>105.9</v>
+      </c>
+      <c r="AC2" s="2" t="n">
+        <v>252.8</v>
+      </c>
+      <c r="AD2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="2" t="n">
+        <v>41.265</v>
+      </c>
+      <c r="AF2" s="2" t="n">
+        <v>56.436</v>
+      </c>
+      <c r="AG2" s="2" t="n">
+        <v>56.374</v>
+      </c>
+      <c r="AH2" s="2" t="n">
+        <v>62.224</v>
+      </c>
+      <c r="AI2" s="2" t="n">
+        <v>59.046</v>
+      </c>
+      <c r="AJ2" s="2" t="n">
+        <v>61.73</v>
+      </c>
+      <c r="AK2" s="2" t="n">
+        <v>50.882</v>
+      </c>
+      <c r="AL2" s="2" t="n">
+        <v>43.052</v>
+      </c>
+      <c r="AM2" s="2" t="n">
+        <v>45.594</v>
+      </c>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+      <c r="BD2" s="2"/>
+      <c r="BE2" s="2"/>
+      <c r="BF2" s="2"/>
+      <c r="BG2" s="2"/>
+      <c r="BH2" s="2"/>
+      <c r="BI2" s="2"/>
+      <c r="BJ2" s="2"/>
+      <c r="BK2" s="2"/>
+      <c r="BL2" s="2"/>
+      <c r="BM2" s="2"/>
+      <c r="BN2" s="2"/>
+      <c r="BO2" s="2"/>
+      <c r="BP2" s="2"/>
+      <c r="BQ2" s="2"/>
+      <c r="BR2" s="2"/>
+      <c r="BS2" s="2"/>
+      <c r="BT2" s="2"/>
+      <c r="BU2" s="2"/>
+      <c r="BV2" s="2"/>
+      <c r="BW2" s="2"/>
+      <c r="BX2" s="2"/>
+      <c r="BY2" s="2"/>
+      <c r="BZ2" s="2"/>
+      <c r="CA2" s="2"/>
+      <c r="CB2" s="2"/>
+      <c r="CC2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>43997.7145949074</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>23.607</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>229.3</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>31.58</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>56.54</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>55.396</v>
+      </c>
+      <c r="S3" s="2" t="n">
+        <v>57.606</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>37.667</v>
+      </c>
+      <c r="U3" s="2" t="n">
+        <v>36.762</v>
+      </c>
+      <c r="V3" s="2" t="n">
+        <v>35.083</v>
+      </c>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2" t="n">
+        <v>41.095</v>
+      </c>
+      <c r="Y3" s="2" t="n">
+        <v>23.901</v>
+      </c>
+      <c r="Z3" s="2" t="n">
+        <v>253.1</v>
+      </c>
+      <c r="AA3" s="2" t="n">
+        <v>0.149</v>
+      </c>
+      <c r="AB3" s="2" t="n">
+        <v>36.7</v>
+      </c>
+      <c r="AC3" s="2" t="n">
+        <v>254.3</v>
+      </c>
+      <c r="AD3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="2" t="n">
+        <v>31.865</v>
+      </c>
+      <c r="AF3" s="2" t="n">
+        <v>56.797</v>
+      </c>
+      <c r="AG3" s="2" t="n">
+        <v>55.617</v>
+      </c>
+      <c r="AH3" s="2" t="n">
+        <v>57.632</v>
+      </c>
+      <c r="AI3" s="2" t="n">
+        <v>37.969</v>
+      </c>
+      <c r="AJ3" s="2" t="n">
+        <v>37.039</v>
+      </c>
+      <c r="AK3" s="2" t="n">
+        <v>35.304</v>
+      </c>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2" t="n">
+        <v>42.098</v>
+      </c>
+      <c r="AN3" s="2" t="n">
+        <v>23.439</v>
+      </c>
+      <c r="AO3" s="2" t="n">
+        <v>207.3</v>
+      </c>
+      <c r="AP3" s="2" t="n">
+        <v>0.181</v>
+      </c>
+      <c r="AQ3" s="2" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="AR3" s="2" t="n">
+        <v>207.5</v>
+      </c>
+      <c r="AS3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="2" t="n">
         <v>31.212</v>
       </c>
-      <c r="Q2" s="2" t="n">
+      <c r="AU3" s="2" t="n">
         <v>56.304</v>
       </c>
-      <c r="R2" s="2" t="n">
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2" t="n">
+        <v>57.598</v>
+      </c>
+      <c r="AX3" s="2" t="n">
+        <v>37.492</v>
+      </c>
+      <c r="AY3" s="2" t="n">
+        <v>36.625</v>
+      </c>
+      <c r="AZ3" s="2" t="n">
+        <v>35.041</v>
+      </c>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2" t="n">
+        <v>23.76</v>
+      </c>
+      <c r="BD3" s="2" t="n">
+        <v>244</v>
+      </c>
+      <c r="BE3" s="2" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="BF3" s="2" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="BG3" s="2" t="n">
+        <v>242.9</v>
+      </c>
+      <c r="BH3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="2" t="n">
+        <v>31.735</v>
+      </c>
+      <c r="BJ3" s="2" t="n">
+        <v>56.638</v>
+      </c>
+      <c r="BK3" s="2"/>
+      <c r="BL3" s="2" t="n">
+        <v>57.655</v>
+      </c>
+      <c r="BM3" s="2" t="n">
+        <v>37.851</v>
+      </c>
+      <c r="BN3" s="2" t="n">
+        <v>36.885</v>
+      </c>
+      <c r="BO3" s="2" t="n">
+        <v>35.273</v>
+      </c>
+      <c r="BP3" s="2"/>
+      <c r="BQ3" s="2"/>
+      <c r="BR3" s="2" t="n">
         <v>55.289</v>
       </c>
-      <c r="S2" s="2" t="n">
-        <v>57.598</v>
-      </c>
-      <c r="T2" s="2" t="n">
-        <v>37.492</v>
-      </c>
-      <c r="U2" s="2" t="n">
-        <v>36.625</v>
-      </c>
-      <c r="V2" s="2" t="n">
+      <c r="BS3" s="2" t="n">
         <v>40.142</v>
       </c>
-      <c r="W2" s="2" t="n">
+      <c r="BT3" s="2" t="n">
         <v>38.508</v>
       </c>
-      <c r="X2" s="2" t="n">
-        <v>35.041</v>
-      </c>
-      <c r="Y2" s="2" t="n">
+      <c r="BU3" s="2" t="n">
         <v>32.833</v>
       </c>
-      <c r="Z2" s="2" t="n">
-        <v>23.607</v>
-      </c>
-      <c r="AA2" s="2" t="n">
-        <v>229.3</v>
-      </c>
-      <c r="AB2" s="2" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="AC2" s="2" t="n">
-        <v>36.9</v>
-      </c>
-      <c r="AD2" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="AE2" s="2" t="n">
+      <c r="BV3" s="2" t="n">
+        <v>39.124</v>
+      </c>
+      <c r="BW3" s="2" t="n">
+        <v>32.934</v>
+      </c>
+      <c r="BX3" s="2" t="n">
+        <v>55.55</v>
+      </c>
+      <c r="BY3" s="2" t="n">
+        <v>41.77</v>
+      </c>
+      <c r="BZ3" s="2" t="n">
+        <v>39.443</v>
+      </c>
+      <c r="CA3" s="2" t="n">
+        <v>33.184</v>
+      </c>
+      <c r="CB3" s="2" t="n">
+        <v>39.645</v>
+      </c>
+      <c r="CC3" s="2" t="n">
+        <v>33.127</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>43906.5528587963</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>21.073</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>229.8</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>0.142</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>230.2</v>
+      </c>
+      <c r="O4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AF2" s="2" t="n">
-        <v>31.58</v>
-      </c>
-      <c r="AG2" s="2" t="n">
-        <v>56.54</v>
-      </c>
-      <c r="AH2" s="2" t="n">
-        <v>55.396</v>
-      </c>
-      <c r="AI2" s="2" t="n">
-        <v>57.606</v>
-      </c>
-      <c r="AJ2" s="2" t="n">
-        <v>37.667</v>
-      </c>
-      <c r="AK2" s="2" t="n">
-        <v>36.762</v>
-      </c>
-      <c r="AL2" s="2" t="n">
-        <v>41.095</v>
-      </c>
-      <c r="AM2" s="2" t="n">
-        <v>39.124</v>
-      </c>
-      <c r="AN2" s="2" t="n">
-        <v>35.083</v>
-      </c>
-      <c r="AO2" s="2" t="n">
-        <v>32.934</v>
-      </c>
-      <c r="AP2" s="2" t="n">
-        <v>23.76</v>
-      </c>
-      <c r="AQ2" s="2" t="n">
-        <v>244</v>
-      </c>
-      <c r="AR2" s="2" t="n">
+      <c r="P4" s="2" t="n">
+        <v>25.241</v>
+      </c>
+      <c r="Q4" s="2" t="n">
+        <v>31.186</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="n">
+        <v>50.335</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <v>37.284</v>
+      </c>
+      <c r="U4" s="2" t="n">
+        <v>39.182</v>
+      </c>
+      <c r="V4" s="2" t="n">
+        <v>35.88</v>
+      </c>
+      <c r="W4" s="2" t="n">
+        <v>33.817</v>
+      </c>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2" t="n">
+        <v>21.062</v>
+      </c>
+      <c r="Z4" s="2" t="n">
+        <v>254.7</v>
+      </c>
+      <c r="AA4" s="2" t="n">
+        <v>0.129</v>
+      </c>
+      <c r="AB4" s="2" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="AC4" s="2" t="n">
+        <v>253.5</v>
+      </c>
+      <c r="AD4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="2" t="n">
+        <v>25.315</v>
+      </c>
+      <c r="AF4" s="2" t="n">
+        <v>31.374</v>
+      </c>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2" t="n">
+        <v>50.422</v>
+      </c>
+      <c r="AI4" s="2" t="n">
+        <v>37.336</v>
+      </c>
+      <c r="AJ4" s="2" t="n">
+        <v>39.232</v>
+      </c>
+      <c r="AK4" s="2" t="n">
+        <v>36.003</v>
+      </c>
+      <c r="AL4" s="2" t="n">
+        <v>33.877</v>
+      </c>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2" t="n">
+        <v>21.065</v>
+      </c>
+      <c r="AO4" s="2" t="n">
+        <v>209.1</v>
+      </c>
+      <c r="AP4" s="2" t="n">
         <v>0.155</v>
       </c>
-      <c r="AS2" s="2" t="n">
-        <v>36.9</v>
-      </c>
-      <c r="AT2" s="2" t="n">
-        <v>242.9</v>
-      </c>
-      <c r="AU2" s="2" t="n">
+      <c r="AQ4" s="2" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="AR4" s="2" t="n">
+        <v>208.4</v>
+      </c>
+      <c r="AS4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AV2" s="2" t="n">
-        <v>31.735</v>
-      </c>
-      <c r="AW2" s="2" t="n">
-        <v>56.638</v>
-      </c>
-      <c r="AX2" s="2" t="n">
-        <v>55.55</v>
-      </c>
-      <c r="AY2" s="2" t="n">
-        <v>57.655</v>
-      </c>
-      <c r="AZ2" s="2" t="n">
-        <v>37.851</v>
-      </c>
-      <c r="BA2" s="2" t="n">
-        <v>36.885</v>
-      </c>
-      <c r="BB2" s="2" t="n">
-        <v>41.77</v>
-      </c>
-      <c r="BC2" s="2" t="n">
-        <v>39.443</v>
-      </c>
-      <c r="BD2" s="2" t="n">
-        <v>35.273</v>
-      </c>
-      <c r="BE2" s="2" t="n">
-        <v>33.184</v>
-      </c>
-      <c r="BF2" s="2" t="n">
-        <v>23.901</v>
-      </c>
-      <c r="BG2" s="2" t="n">
-        <v>253.1</v>
-      </c>
-      <c r="BH2" s="2" t="n">
-        <v>0.149</v>
-      </c>
-      <c r="BI2" s="2" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="BJ2" s="2" t="n">
-        <v>254.3</v>
-      </c>
-      <c r="BK2" s="2" t="n">
+      <c r="AT4" s="2" t="n">
+        <v>24.961</v>
+      </c>
+      <c r="AU4" s="2" t="n">
+        <v>30.773</v>
+      </c>
+      <c r="AV4" s="2" t="n">
+        <v>34.277</v>
+      </c>
+      <c r="AW4" s="2" t="n">
+        <v>49.996</v>
+      </c>
+      <c r="AX4" s="2" t="n">
+        <v>37.057</v>
+      </c>
+      <c r="AY4" s="2" t="n">
+        <v>38.944</v>
+      </c>
+      <c r="AZ4" s="2" t="n">
+        <v>35.411</v>
+      </c>
+      <c r="BA4" s="2" t="n">
+        <v>33.479</v>
+      </c>
+      <c r="BB4" s="2" t="n">
+        <v>34.643</v>
+      </c>
+      <c r="BC4" s="2" t="n">
+        <v>21.069</v>
+      </c>
+      <c r="BD4" s="2" t="n">
+        <v>243.4</v>
+      </c>
+      <c r="BE4" s="2" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="BF4" s="2" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="BG4" s="2" t="n">
+        <v>244.4</v>
+      </c>
+      <c r="BH4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BL2" s="2" t="n">
-        <v>31.865</v>
-      </c>
-      <c r="BM2" s="2" t="n">
-        <v>56.797</v>
-      </c>
-      <c r="BN2" s="2" t="n">
-        <v>55.617</v>
-      </c>
-      <c r="BO2" s="2" t="n">
-        <v>57.632</v>
-      </c>
-      <c r="BP2" s="2" t="n">
-        <v>37.969</v>
-      </c>
-      <c r="BQ2" s="2" t="n">
-        <v>37.039</v>
-      </c>
-      <c r="BR2" s="2" t="n">
-        <v>42.098</v>
-      </c>
-      <c r="BS2" s="2" t="n">
-        <v>39.645</v>
-      </c>
-      <c r="BT2" s="2" t="n">
-        <v>35.304</v>
-      </c>
-      <c r="BU2" s="2" t="n">
-        <v>33.127</v>
-      </c>
+      <c r="BI4" s="2" t="n">
+        <v>25.351</v>
+      </c>
+      <c r="BJ4" s="2" t="n">
+        <v>31.318</v>
+      </c>
+      <c r="BK4" s="2" t="n">
+        <v>34.758</v>
+      </c>
+      <c r="BL4" s="2" t="n">
+        <v>50.44</v>
+      </c>
+      <c r="BM4" s="2" t="n">
+        <v>37.286</v>
+      </c>
+      <c r="BN4" s="2" t="n">
+        <v>39.22</v>
+      </c>
+      <c r="BO4" s="2" t="n">
+        <v>35.95</v>
+      </c>
+      <c r="BP4" s="2" t="n">
+        <v>33.863</v>
+      </c>
+      <c r="BQ4" s="2" t="n">
+        <v>34.789</v>
+      </c>
+      <c r="BR4" s="2"/>
+      <c r="BS4" s="2"/>
+      <c r="BT4" s="2"/>
+      <c r="BU4" s="2"/>
+      <c r="BV4" s="2"/>
+      <c r="BW4" s="2"/>
+      <c r="BX4" s="2"/>
+      <c r="BY4" s="2"/>
+      <c r="BZ4" s="2"/>
+      <c r="CA4" s="2"/>
+      <c r="CB4" s="2"/>
+      <c r="CC4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>